<commit_message>
Fixed the expense download
</commit_message>
<xml_diff>
--- a/TechParvaLEAO/Uploads/DownloadTemplate (2).xlsx
+++ b/TechParvaLEAO/Uploads/DownloadTemplate (2).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\priya.mishra\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99CDC19E-0746-4DB2-8F7D-0D25DE50CCB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01F1F7CA-06B8-42FF-80A2-D9AF5C9CF258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4037" uniqueCount="2122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4029" uniqueCount="2117">
   <si>
     <t>Employee Code</t>
   </si>
@@ -6374,25 +6374,10 @@
     <t>YES</t>
   </si>
   <si>
-    <t>test n2</t>
-  </si>
-  <si>
-    <t>test n3</t>
-  </si>
-  <si>
-    <t>C536072024n7</t>
-  </si>
-  <si>
-    <t>C536072024n8</t>
-  </si>
-  <si>
-    <t>C536072024n9</t>
-  </si>
-  <si>
     <t>M</t>
   </si>
   <si>
-    <t>F</t>
+    <t>C536072024n28</t>
   </si>
 </sst>
 </file>
@@ -6440,7 +6425,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -6463,24 +6448,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -6503,32 +6475,21 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="23">
+    <dxf>
+      <font>
+        <color indexed="20"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="45"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color indexed="20"/>
@@ -7243,16 +7204,6 @@
         <horizontal/>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <color indexed="20"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="45"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -7267,29 +7218,29 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:T4" totalsRowShown="0" dataDxfId="1">
-  <autoFilter ref="A1:T4" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:T2" totalsRowShown="0" dataDxfId="2">
+  <autoFilter ref="A1:T2" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="20">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Employee Code" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Employee" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Designation" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Location" dataDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Authorization Profile" dataDxfId="17"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Expense Profile" dataDxfId="16"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Teams" dataDxfId="15"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Account Number" dataDxfId="14"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Reporting To" dataDxfId="13"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Email" dataDxfId="12"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Gender" dataDxfId="11"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Date Of Joining" dataDxfId="10"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Date Of Birth" dataDxfId="9"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Overtime Rule" dataDxfId="8"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Can Apply Mission Leaves" dataDxfId="7"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Can Create Forex Requests" dataDxfId="6"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Can have Credit Card" dataDxfId="5"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Is Hr" dataDxfId="4"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="On Field Employee" dataDxfId="3"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Specific Weekly-Off" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Employee Code" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Employee" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Designation" dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Location" dataDxfId="19"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Authorization Profile" dataDxfId="18"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Expense Profile" dataDxfId="17"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Teams" dataDxfId="16"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Account Number" dataDxfId="15"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Reporting To" dataDxfId="14"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Email" dataDxfId="13"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Gender" dataDxfId="12"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Date Of Joining" dataDxfId="11"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Date Of Birth" dataDxfId="10"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Overtime Rule" dataDxfId="9"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Can Apply Mission Leaves" dataDxfId="8"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Can Create Forex Requests" dataDxfId="7"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Can have Credit Card" dataDxfId="6"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Is Hr" dataDxfId="5"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="On Field Employee" dataDxfId="4"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Specific Weekly-Off" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7661,10 +7612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T4"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A3" sqref="A3:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7733,7 +7684,7 @@
     </row>
     <row r="2" spans="1:20" ht="108">
       <c r="A2" s="1" t="s">
-        <v>2117</v>
+        <v>2116</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2105</v>
@@ -7763,7 +7714,7 @@
         <v>2112</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>2120</v>
+        <v>2115</v>
       </c>
       <c r="L2" s="6">
         <v>45139</v>
@@ -7787,74 +7738,10 @@
         <v>2114</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="18">
-      <c r="A3" s="1" t="s">
-        <v>2118</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>2115</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="3">
-        <v>123456</v>
-      </c>
-      <c r="I3" s="3"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="3" t="s">
-        <v>2121</v>
-      </c>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="3"/>
-      <c r="S3" s="3"/>
-      <c r="T3" s="7"/>
-    </row>
-    <row r="4" spans="1:20" ht="18">
-      <c r="A4" s="8" t="s">
-        <v>2119</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>2116</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="3">
-        <v>123456</v>
-      </c>
-      <c r="I4" s="10"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="10" t="s">
-        <v>2121</v>
-      </c>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="10"/>
-      <c r="S4" s="10"/>
-      <c r="T4" s="14"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:A4">
-    <cfRule type="expression" dxfId="22" priority="1" stopIfTrue="1">
-      <formula>AND(COUNTIF($B$1:$B$2141, A2)+COUNTIF($B$2160:$B$65514, A2)+COUNTIF($B$2146:$B$2152, A2)&gt;1,NOT(ISBLANK(A2)))</formula>
+  <conditionalFormatting sqref="A2">
+    <cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1">
+      <formula>AND(COUNTIF($B$1:$B$2139, A2)+COUNTIF($B$2158:$B$65512, A2)+COUNTIF($B$2144:$B$2150, A2)&gt;1,NOT(ISBLANK(A2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>